<commit_message>
Se actualizo la lista de paquetes
</commit_message>
<xml_diff>
--- a/util/paquetes.xlsx
+++ b/util/paquetes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">PAQUETES</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t xml:space="preserve">caTools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visdat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tidymodels</t>
   </si>
   <si>
     <t xml:space="preserve">dplyr</t>
@@ -241,12 +247,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,13 +281,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
   </cols>
@@ -510,6 +520,16 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>